<commit_message>
Datasets without atypicals + consensus pocket selection
</commit_message>
<xml_diff>
--- a/data/Type_II_abundance.xlsx
+++ b/data/Type_II_abundance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="4040" windowWidth="33760" windowHeight="22340"/>
+    <workbookView xWindow="16700" yWindow="4040" windowWidth="33760" windowHeight="22340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="98">
   <si>
     <t>KLIFS position</t>
   </si>
@@ -305,6 +305,15 @@
   </si>
   <si>
     <t>a.l.85</t>
+  </si>
+  <si>
+    <t>MAX contacts (BB or SC)</t>
+  </si>
+  <si>
+    <t>Matches</t>
+  </si>
+  <si>
+    <t>Abundance cutoff</t>
   </si>
 </sst>
 </file>
@@ -370,14 +379,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -389,12 +408,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -726,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -2329,19 +2359,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="N1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="10" width="6.1640625" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" customWidth="1"/>
+    <col min="17" max="17" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="151">
+    <row r="1" spans="1:18" ht="151">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2372,8 +2404,11 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="N1" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2413,8 +2448,22 @@
         <f>IF(ISBLANK(Counts!J2),"-", Counts!J2/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="N2" s="4">
+        <f>MAX(C2,H2)</f>
+        <v>2.1367521367521368E-2</v>
+      </c>
+      <c r="O2" s="3" t="str">
+        <f>IF(N2&gt;=R$2,A2,"")</f>
+        <v/>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2454,8 +2503,23 @@
         <f>IF(ISBLANK(Counts!J3),"-", Counts!J3/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="N3" s="4">
+        <f t="shared" ref="N3:N66" si="0">MAX(C3,H3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="str">
+        <f t="shared" ref="O3:O66" si="1">IF(N3&gt;=R$2,A3,"")</f>
+        <v/>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3">
+        <f>COUNTIF(O2:O86,"*.*")</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2495,8 +2559,16 @@
         <f>IF(ISBLANK(Counts!J4),"-", Counts!J4/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="N4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="O4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>I.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -2536,8 +2608,16 @@
         <f>IF(ISBLANK(Counts!J5),"-", Counts!J5/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="N5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="O5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>g.l.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2577,8 +2657,16 @@
         <f>IF(ISBLANK(Counts!J6),"-", Counts!J6/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="N6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="O6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2618,8 +2706,16 @@
         <f>IF(ISBLANK(Counts!J7),"-", Counts!J7/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="N7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="O7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2659,8 +2755,16 @@
         <f>IF(ISBLANK(Counts!J8),"-", Counts!J8/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="N8" s="4">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="O8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2700,8 +2804,16 @@
         <f>IF(ISBLANK(Counts!J9),"-", Counts!J9/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="N9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15811965811965811</v>
+      </c>
+      <c r="O9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>g.l.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -2741,8 +2853,16 @@
         <f>IF(ISBLANK(Counts!J10),"-", Counts!J10/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="N10" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1367521367521368E-2</v>
+      </c>
+      <c r="O10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -2782,8 +2902,16 @@
         <f>IF(ISBLANK(Counts!J11),"-", Counts!J11/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="N11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+      <c r="O11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -2823,8 +2951,16 @@
         <f>IF(ISBLANK(Counts!J12),"-", Counts!J12/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="N12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95726495726495731</v>
+      </c>
+      <c r="O12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>II.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -2864,8 +3000,16 @@
         <f>IF(ISBLANK(Counts!J13),"-", Counts!J13/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="N13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.13675213675213677</v>
+      </c>
+      <c r="O13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>II.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2905,8 +3049,16 @@
         <f>IF(ISBLANK(Counts!J14),"-", Counts!J14/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="N14" s="4">
+        <f t="shared" si="0"/>
+        <v>5.9829059829059832E-2</v>
+      </c>
+      <c r="O14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>II.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2946,8 +3098,16 @@
         <f>IF(ISBLANK(Counts!J15),"-", Counts!J15/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="N15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -2987,8 +3147,16 @@
         <f>IF(ISBLANK(Counts!J16),"-", Counts!J16/234)</f>
         <v>4.2735042735042739E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="N16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95726495726495731</v>
+      </c>
+      <c r="O16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>III.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -3028,8 +3196,16 @@
         <f>IF(ISBLANK(Counts!J17),"-", Counts!J17/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="N17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.48717948717948717</v>
+      </c>
+      <c r="O17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>III.16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -3069,8 +3245,16 @@
         <f>IF(ISBLANK(Counts!J18),"-", Counts!J18/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="N18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95726495726495731</v>
+      </c>
+      <c r="O18" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>III.17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -3110,8 +3294,16 @@
         <f>IF(ISBLANK(Counts!J19),"-", Counts!J19/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="N19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -3151,8 +3343,16 @@
         <f>IF(ISBLANK(Counts!J20),"-", Counts!J20/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="N20" s="4">
+        <f t="shared" si="0"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="O20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -3192,8 +3392,16 @@
         <f>IF(ISBLANK(Counts!J21),"-", Counts!J21/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="N21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="O21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3233,8 +3441,16 @@
         <f>IF(ISBLANK(Counts!J22),"-", Counts!J22/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="N22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.10683760683760683</v>
+      </c>
+      <c r="O22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -3274,8 +3490,16 @@
         <f>IF(ISBLANK(Counts!J23),"-", Counts!J23/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="N23" s="4">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="O23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -3315,8 +3539,16 @@
         <f>IF(ISBLANK(Counts!J24),"-", Counts!J24/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="N24" s="4">
+        <f t="shared" si="0"/>
+        <v>0.1623931623931624</v>
+      </c>
+      <c r="O24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -3356,8 +3588,16 @@
         <f>IF(ISBLANK(Counts!J25),"-", Counts!J25/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="N25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.89316239316239321</v>
+      </c>
+      <c r="O25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -3397,8 +3637,16 @@
         <f>IF(ISBLANK(Counts!J26),"-", Counts!J26/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="N26" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14102564102564102</v>
+      </c>
+      <c r="O26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -3438,8 +3686,16 @@
         <f>IF(ISBLANK(Counts!J27),"-", Counts!J27/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="N27" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -3479,8 +3735,16 @@
         <f>IF(ISBLANK(Counts!J28),"-", Counts!J28/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="N28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.74786324786324787</v>
+      </c>
+      <c r="O28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -3520,8 +3784,16 @@
         <f>IF(ISBLANK(Counts!J29),"-", Counts!J29/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="N29" s="4">
+        <f t="shared" si="0"/>
+        <v>0.94871794871794868</v>
+      </c>
+      <c r="O29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αC.28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -3561,8 +3833,16 @@
         <f>IF(ISBLANK(Counts!J30),"-", Counts!J30/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="N30" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -3602,8 +3882,16 @@
         <f>IF(ISBLANK(Counts!J31),"-", Counts!J31/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="N31" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -3643,8 +3931,16 @@
         <f>IF(ISBLANK(Counts!J32),"-", Counts!J32/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="N32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.8504273504273504</v>
+      </c>
+      <c r="O32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>b.l.31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -3684,8 +3980,16 @@
         <f>IF(ISBLANK(Counts!J33),"-", Counts!J33/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="N33" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -3725,8 +4029,16 @@
         <f>IF(ISBLANK(Counts!J34),"-", Counts!J34/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="N34" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
@@ -3766,8 +4078,16 @@
         <f>IF(ISBLANK(Counts!J35),"-", Counts!J35/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="N35" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
@@ -3807,8 +4127,16 @@
         <f>IF(ISBLANK(Counts!J36),"-", Counts!J36/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="N36" s="4">
+        <f t="shared" si="0"/>
+        <v>0.82478632478632474</v>
+      </c>
+      <c r="O36" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>b.l.35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
@@ -3848,8 +4176,16 @@
         <f>IF(ISBLANK(Counts!J37),"-", Counts!J37/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="N37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95726495726495731</v>
+      </c>
+      <c r="O37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>b.l.36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -3889,8 +4225,16 @@
         <f>IF(ISBLANK(Counts!J38),"-", Counts!J38/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="N38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.12820512820512819</v>
+      </c>
+      <c r="O38" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>b.l.37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -3930,8 +4274,16 @@
         <f>IF(ISBLANK(Counts!J39),"-", Counts!J39/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="N39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.21367521367521367</v>
+      </c>
+      <c r="O39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IV.38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -3971,8 +4323,16 @@
         <f>IF(ISBLANK(Counts!J40),"-", Counts!J40/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="N40" s="4">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+      <c r="O40" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -4012,8 +4372,16 @@
         <f>IF(ISBLANK(Counts!J41),"-", Counts!J41/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="N41" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1367521367521368E-2</v>
+      </c>
+      <c r="O41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -4053,8 +4421,16 @@
         <f>IF(ISBLANK(Counts!J42),"-", Counts!J42/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="N42" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -4094,8 +4470,16 @@
         <f>IF(ISBLANK(Counts!J43),"-", Counts!J43/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="N43" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -4135,8 +4519,16 @@
         <f>IF(ISBLANK(Counts!J44),"-", Counts!J44/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="N44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.80341880341880345</v>
+      </c>
+      <c r="O44" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>V.43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -4176,8 +4568,16 @@
         <f>IF(ISBLANK(Counts!J45),"-", Counts!J45/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="N45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.17094017094017094</v>
+      </c>
+      <c r="O45" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>V.44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -4217,8 +4617,16 @@
         <f>IF(ISBLANK(Counts!J46),"-", Counts!J46/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="N46" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95726495726495731</v>
+      </c>
+      <c r="O46" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>GK.45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -4258,8 +4666,16 @@
         <f>IF(ISBLANK(Counts!J47),"-", Counts!J47/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="N47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.6495726495726496</v>
+      </c>
+      <c r="O47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>hinge.46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -4299,8 +4715,16 @@
         <f>IF(ISBLANK(Counts!J48),"-", Counts!J48/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="N48" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9145299145299145</v>
+      </c>
+      <c r="O48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>hinge.47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
@@ -4340,8 +4764,16 @@
         <f>IF(ISBLANK(Counts!J49),"-", Counts!J49/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="N49" s="4">
+        <f t="shared" si="0"/>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="O49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>hinge.48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -4381,8 +4813,16 @@
         <f>IF(ISBLANK(Counts!J50),"-", Counts!J50/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="N50" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31196581196581197</v>
+      </c>
+      <c r="O50" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>linker.49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
@@ -4422,8 +4862,16 @@
         <f>IF(ISBLANK(Counts!J51),"-", Counts!J51/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="N51" s="4">
+        <f t="shared" si="0"/>
+        <v>0.42307692307692307</v>
+      </c>
+      <c r="O51" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>linker.50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -4463,8 +4911,16 @@
         <f>IF(ISBLANK(Counts!J52),"-", Counts!J52/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="N52" s="4">
+        <f t="shared" si="0"/>
+        <v>0.64529914529914534</v>
+      </c>
+      <c r="O52" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>linker.51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -4504,8 +4960,16 @@
         <f>IF(ISBLANK(Counts!J53),"-", Counts!J53/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="N53" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23504273504273504</v>
+      </c>
+      <c r="O53" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>linker.52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -4545,8 +5009,16 @@
         <f>IF(ISBLANK(Counts!J54),"-", Counts!J54/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="N54" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O54" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
@@ -4586,8 +5058,16 @@
         <f>IF(ISBLANK(Counts!J55),"-", Counts!J55/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="N55" s="4">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+      <c r="O55" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -4627,8 +5107,16 @@
         <f>IF(ISBLANK(Counts!J56),"-", Counts!J56/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="N56" s="4">
+        <f t="shared" si="0"/>
+        <v>0.12820512820512819</v>
+      </c>
+      <c r="O56" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αD.55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -4668,8 +5156,16 @@
         <f>IF(ISBLANK(Counts!J57),"-", Counts!J57/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="N57" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O57" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
@@ -4709,8 +5205,16 @@
         <f>IF(ISBLANK(Counts!J58),"-", Counts!J58/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="N58" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O58" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
@@ -4750,8 +5254,16 @@
         <f>IF(ISBLANK(Counts!J59),"-", Counts!J59/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="N59" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O59" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -4791,8 +5303,16 @@
         <f>IF(ISBLANK(Counts!J60),"-", Counts!J60/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="N60" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O60" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -4832,8 +5352,16 @@
         <f>IF(ISBLANK(Counts!J61),"-", Counts!J61/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="N61" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O61" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
@@ -4873,8 +5401,16 @@
         <f>IF(ISBLANK(Counts!J62),"-", Counts!J62/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="N62" s="4">
+        <f t="shared" si="0"/>
+        <v>0.80769230769230771</v>
+      </c>
+      <c r="O62" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>αE.61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -4914,8 +5450,16 @@
         <f>IF(ISBLANK(Counts!J63),"-", Counts!J63/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="N63" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O63" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="1" t="s">
         <v>72</v>
       </c>
@@ -4955,8 +5499,16 @@
         <f>IF(ISBLANK(Counts!J64),"-", Counts!J64/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="N64" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O64" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="1" t="s">
         <v>73</v>
       </c>
@@ -4996,8 +5548,16 @@
         <f>IF(ISBLANK(Counts!J65),"-", Counts!J65/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="N65" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O65" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
@@ -5037,8 +5597,16 @@
         <f>IF(ISBLANK(Counts!J66),"-", Counts!J66/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="N66" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O66" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="1" t="s">
         <v>75</v>
       </c>
@@ -5078,8 +5646,16 @@
         <f>IF(ISBLANK(Counts!J67),"-", Counts!J67/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="N67" s="4">
+        <f t="shared" ref="N67:N86" si="2">MAX(C67,H67)</f>
+        <v>0.74358974358974361</v>
+      </c>
+      <c r="O67" s="3" t="str">
+        <f t="shared" ref="O67:O86" si="3">IF(N67&gt;=R$2,A67,"")</f>
+        <v>VI.66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -5119,8 +5695,16 @@
         <f>IF(ISBLANK(Counts!J68),"-", Counts!J68/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="N68" s="4">
+        <f t="shared" si="2"/>
+        <v>0.13675213675213677</v>
+      </c>
+      <c r="O68" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>VI.67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
@@ -5160,8 +5744,16 @@
         <f>IF(ISBLANK(Counts!J69),"-", Counts!J69/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="N69" s="4">
+        <f t="shared" si="2"/>
+        <v>0.84188034188034189</v>
+      </c>
+      <c r="O69" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>c.l.68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="1" t="s">
         <v>78</v>
       </c>
@@ -5201,8 +5793,16 @@
         <f>IF(ISBLANK(Counts!J70),"-", Counts!J70/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="N70" s="4">
+        <f t="shared" si="2"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="O70" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>c.l.69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" s="1" t="s">
         <v>79</v>
       </c>
@@ -5242,8 +5842,16 @@
         <f>IF(ISBLANK(Counts!J71),"-", Counts!J71/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="N71" s="4">
+        <f t="shared" si="2"/>
+        <v>2.9914529914529916E-2</v>
+      </c>
+      <c r="O71" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
@@ -5283,8 +5891,16 @@
         <f>IF(ISBLANK(Counts!J72),"-", Counts!J72/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="N72" s="4">
+        <f t="shared" si="2"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="O72" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73" s="1" t="s">
         <v>81</v>
       </c>
@@ -5324,8 +5940,16 @@
         <f>IF(ISBLANK(Counts!J73),"-", Counts!J73/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="N73" s="4">
+        <f t="shared" si="2"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O73" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" s="1" t="s">
         <v>82</v>
       </c>
@@ -5365,8 +5989,16 @@
         <f>IF(ISBLANK(Counts!J74),"-", Counts!J74/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="N74" s="4">
+        <f t="shared" si="2"/>
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="O74" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
@@ -5406,8 +6038,16 @@
         <f>IF(ISBLANK(Counts!J75),"-", Counts!J75/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="N75" s="4">
+        <f t="shared" si="2"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="O75" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>c.l.74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="1" t="s">
         <v>84</v>
       </c>
@@ -5447,8 +6087,16 @@
         <f>IF(ISBLANK(Counts!J76),"-", Counts!J76/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="N76" s="4">
+        <f t="shared" si="2"/>
+        <v>0.13247863247863248</v>
+      </c>
+      <c r="O76" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>c.l.75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" s="1" t="s">
         <v>85</v>
       </c>
@@ -5488,8 +6136,16 @@
         <f>IF(ISBLANK(Counts!J77),"-", Counts!J77/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="N77" s="4">
+        <f t="shared" si="2"/>
+        <v>4.2735042735042736E-2</v>
+      </c>
+      <c r="O77" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" s="1" t="s">
         <v>86</v>
       </c>
@@ -5529,8 +6185,16 @@
         <f>IF(ISBLANK(Counts!J78),"-", Counts!J78/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="N78" s="4">
+        <f t="shared" si="2"/>
+        <v>0.86324786324786329</v>
+      </c>
+      <c r="O78" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>VII.77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="1" t="s">
         <v>87</v>
       </c>
@@ -5570,8 +6234,16 @@
         <f>IF(ISBLANK(Counts!J79),"-", Counts!J79/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="80" spans="1:10">
+      <c r="N79" s="4">
+        <f t="shared" si="2"/>
+        <v>5.9829059829059832E-2</v>
+      </c>
+      <c r="O79" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>VII.78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" s="1" t="s">
         <v>88</v>
       </c>
@@ -5611,8 +6283,16 @@
         <f>IF(ISBLANK(Counts!J80),"-", Counts!J80/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="81" spans="1:10">
+      <c r="N80" s="4">
+        <f t="shared" si="2"/>
+        <v>0.79914529914529919</v>
+      </c>
+      <c r="O80" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>VIII.79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="1" t="s">
         <v>89</v>
       </c>
@@ -5652,8 +6332,16 @@
         <f>IF(ISBLANK(Counts!J81),"-", Counts!J81/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="N81" s="4">
+        <f t="shared" si="2"/>
+        <v>0.87179487179487181</v>
+      </c>
+      <c r="O81" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>xDFG.80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="1" t="s">
         <v>90</v>
       </c>
@@ -5693,8 +6381,16 @@
         <f>IF(ISBLANK(Counts!J82),"-", Counts!J82/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="N82" s="4">
+        <f t="shared" si="2"/>
+        <v>0.90598290598290598</v>
+      </c>
+      <c r="O82" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>xDFG.81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="1" t="s">
         <v>91</v>
       </c>
@@ -5734,8 +6430,16 @@
         <f>IF(ISBLANK(Counts!J83),"-", Counts!J83/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="N83" s="4">
+        <f t="shared" si="2"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="O83" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>xDFG.82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="1" t="s">
         <v>92</v>
       </c>
@@ -5775,8 +6479,16 @@
         <f>IF(ISBLANK(Counts!J84),"-", Counts!J84/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="N84" s="4">
+        <f t="shared" si="2"/>
+        <v>0.29059829059829062</v>
+      </c>
+      <c r="O84" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>xDFG.83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="1" t="s">
         <v>93</v>
       </c>
@@ -5816,8 +6528,16 @@
         <f>IF(ISBLANK(Counts!J85),"-", Counts!J85/234)</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="N85" s="4">
+        <f t="shared" si="2"/>
+        <v>0.18376068376068377</v>
+      </c>
+      <c r="O85" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>a.l.84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" s="1" t="s">
         <v>94</v>
       </c>
@@ -5857,14 +6577,34 @@
         <f>IF(ISBLANK(Counts!J86),"-", Counts!J86/234)</f>
         <v>-</v>
       </c>
+      <c r="N86" s="4">
+        <f t="shared" si="2"/>
+        <v>7.2649572649572655E-2</v>
+      </c>
+      <c r="O86" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>a.l.85</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:J86">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N86">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>

</xml_diff>

<commit_message>
Renamed contact to proximity
</commit_message>
<xml_diff>
--- a/data/Type_II_abundance.xlsx
+++ b/data/Type_II_abundance.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/kinometree/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE17DF1-A990-2749-895F-627E4B96214B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="4040" windowWidth="33760" windowHeight="22340" activeTab="1"/>
+    <workbookView xWindow="6160" yWindow="9380" windowWidth="33760" windowHeight="22340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
     <sheet name="Frequencies" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,9 +34,6 @@
     <t>Aromatic_sidechain</t>
   </si>
   <si>
-    <t>Contact_sidechain</t>
-  </si>
-  <si>
     <t>H-bond_sidechain</t>
   </si>
   <si>
@@ -43,9 +46,6 @@
     <t>Halogen bond_sidechain</t>
   </si>
   <si>
-    <t>Contact_backbone</t>
-  </si>
-  <si>
     <t>H-bond_backbone</t>
   </si>
   <si>
@@ -314,12 +314,18 @@
   </si>
   <si>
     <t>Abundance cutoff</t>
+  </si>
+  <si>
+    <t>Proximity_backbone</t>
+  </si>
+  <si>
+    <t>Proximity_sidechain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -429,6 +435,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -753,14 +767,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="6" width="4.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -769,7 +783,7 @@
     <col min="10" max="10" width="4.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="151">
+    <row r="1" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -777,33 +791,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
@@ -824,14 +838,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3">
         <v>216</v>
@@ -846,9 +860,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H5" s="3">
         <v>27</v>
@@ -857,9 +871,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -880,9 +894,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" s="3">
         <v>9</v>
@@ -891,9 +905,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>6</v>
@@ -911,9 +925,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3">
         <v>26</v>
@@ -934,9 +948,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H10" s="3">
         <v>5</v>
@@ -945,9 +959,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -962,9 +976,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3">
         <v>224</v>
@@ -979,9 +993,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -996,9 +1010,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -1022,9 +1036,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1039,9 +1053,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
         <v>224</v>
@@ -1059,9 +1073,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1076,9 +1090,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3">
         <v>224</v>
@@ -1099,9 +1113,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1116,9 +1130,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="3">
         <v>9</v>
@@ -1127,9 +1141,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3">
         <v>18</v>
@@ -1144,9 +1158,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -1164,9 +1178,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -1181,9 +1195,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3">
         <v>34</v>
@@ -1201,9 +1215,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3">
         <v>209</v>
@@ -1224,9 +1238,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3">
         <v>11</v>
@@ -1241,9 +1255,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -1258,9 +1272,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3">
         <v>175</v>
@@ -1275,9 +1289,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="3">
         <v>222</v>
@@ -1295,9 +1309,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -1312,9 +1326,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
@@ -1329,9 +1343,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3">
         <v>25</v>
@@ -1352,37 +1366,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1</v>
-      </c>
-      <c r="I33" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3">
-        <v>1</v>
-      </c>
-      <c r="H34" s="3">
-        <v>1</v>
-      </c>
-      <c r="I34" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
@@ -1397,9 +1411,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
@@ -1417,9 +1431,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" s="3">
         <v>224</v>
@@ -1434,9 +1448,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -1451,9 +1465,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" s="3">
         <v>50</v>
@@ -1462,9 +1476,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -1479,9 +1493,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H41" s="3">
         <v>5</v>
@@ -1490,9 +1504,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" s="3">
         <v>2</v>
@@ -1507,9 +1521,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -1524,9 +1538,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="3">
         <v>188</v>
@@ -1541,9 +1555,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -1558,9 +1572,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B46" s="3">
         <v>17</v>
@@ -1581,9 +1595,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" s="3">
         <v>69</v>
@@ -1604,9 +1618,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B48" s="3">
         <v>116</v>
@@ -1627,9 +1641,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B49" s="3">
         <v>2</v>
@@ -1650,9 +1664,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C50" s="3">
         <v>19</v>
@@ -1673,9 +1687,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C51" s="3">
         <v>3</v>
@@ -1690,9 +1704,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" s="3">
         <v>4</v>
@@ -1707,9 +1721,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C53" s="3">
         <v>55</v>
@@ -1730,9 +1744,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C54" s="3">
         <v>1</v>
@@ -1747,9 +1761,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C55" s="3">
         <v>3</v>
@@ -1764,9 +1778,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C56" s="3">
         <v>30</v>
@@ -1787,9 +1801,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C57" s="3">
         <v>2</v>
@@ -1804,9 +1818,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C58" s="3">
         <v>1</v>
@@ -1821,9 +1835,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C59" s="3">
         <v>2</v>
@@ -1838,9 +1852,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C60" s="3">
         <v>2</v>
@@ -1855,9 +1869,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B61" s="3">
         <v>1</v>
@@ -1875,9 +1889,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C62" s="3">
         <v>189</v>
@@ -1892,71 +1906,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="H63" s="3">
+        <v>1</v>
+      </c>
+      <c r="I63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+      <c r="D64" s="3">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C63" s="3">
-        <v>1</v>
-      </c>
-      <c r="E63" s="3">
-        <v>1</v>
-      </c>
-      <c r="H63" s="3">
-        <v>1</v>
-      </c>
-      <c r="I63" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1" t="s">
+      <c r="C65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3">
+        <v>1</v>
+      </c>
+      <c r="H65" s="3">
+        <v>1</v>
+      </c>
+      <c r="I65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C64" s="3">
-        <v>1</v>
-      </c>
-      <c r="D64" s="3">
-        <v>1</v>
-      </c>
-      <c r="H64" s="3">
-        <v>1</v>
-      </c>
-      <c r="I64" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="1" t="s">
+      <c r="H66" s="3">
+        <v>1</v>
+      </c>
+      <c r="I66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C65" s="3">
-        <v>1</v>
-      </c>
-      <c r="E65" s="3">
-        <v>1</v>
-      </c>
-      <c r="H65" s="3">
-        <v>1</v>
-      </c>
-      <c r="I65" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H66" s="3">
-        <v>1</v>
-      </c>
-      <c r="I66" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="B67" s="3">
         <v>36</v>
@@ -1977,9 +1991,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C68" s="3">
         <v>23</v>
@@ -1994,9 +2008,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B69" s="3">
         <v>16</v>
@@ -2020,9 +2034,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C70" s="3">
         <v>27</v>
@@ -2043,9 +2057,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C71" s="3">
         <v>4</v>
@@ -2063,9 +2077,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C72" s="3">
         <v>2</v>
@@ -2077,43 +2091,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="3">
+        <v>1</v>
+      </c>
+      <c r="E73" s="3">
+        <v>1</v>
+      </c>
+      <c r="H73" s="3">
+        <v>1</v>
+      </c>
+      <c r="I73" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="3">
+        <v>1</v>
+      </c>
+      <c r="E74" s="3">
+        <v>1</v>
+      </c>
+      <c r="H74" s="3">
+        <v>1</v>
+      </c>
+      <c r="I74" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C73" s="3">
-        <v>1</v>
-      </c>
-      <c r="E73" s="3">
-        <v>1</v>
-      </c>
-      <c r="H73" s="3">
-        <v>1</v>
-      </c>
-      <c r="I73" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C74" s="3">
-        <v>1</v>
-      </c>
-      <c r="E74" s="3">
-        <v>1</v>
-      </c>
-      <c r="H74" s="3">
-        <v>1</v>
-      </c>
-      <c r="I74" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C75" s="3">
         <v>2</v>
@@ -2131,9 +2145,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C76" s="3">
         <v>12</v>
@@ -2148,9 +2162,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C77" s="3">
         <v>1</v>
@@ -2165,9 +2179,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B78" s="3">
         <v>21</v>
@@ -2185,9 +2199,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C79" s="3">
         <v>1</v>
@@ -2202,9 +2216,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C80" s="3">
         <v>171</v>
@@ -2219,9 +2233,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C81" s="3">
         <v>164</v>
@@ -2239,9 +2253,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C82" s="3">
         <v>212</v>
@@ -2262,9 +2276,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B83" s="3">
         <v>193</v>
@@ -2282,9 +2296,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H84" s="3">
         <v>68</v>
@@ -2293,9 +2307,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B85" s="3">
         <v>2</v>
@@ -2316,9 +2330,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C86" s="3">
         <v>17</v>
@@ -2358,14 +2372,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="N1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="10" width="6.1640625" customWidth="1"/>
@@ -2373,7 +2387,7 @@
     <col min="17" max="17" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="151">
+    <row r="1" spans="1:18" ht="160" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2381,36 +2395,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>IF(ISBLANK(Counts!B2),"-", Counts!B2/234)</f>
@@ -2457,15 +2471,15 @@
         <v/>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R2" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>IF(ISBLANK(Counts!B3),"-", Counts!B3/234)</f>
@@ -2512,16 +2526,16 @@
         <v/>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R3">
         <f>COUNTIF(O2:O86,"*.*")</f>
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>IF(ISBLANK(Counts!B4),"-", Counts!B4/234)</f>
@@ -2568,9 +2582,9 @@
         <v>I.3</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>IF(ISBLANK(Counts!B5),"-", Counts!B5/234)</f>
@@ -2617,9 +2631,9 @@
         <v>g.l.4</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>IF(ISBLANK(Counts!B6),"-", Counts!B6/234)</f>
@@ -2666,9 +2680,9 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>IF(ISBLANK(Counts!B7),"-", Counts!B7/234)</f>
@@ -2715,9 +2729,9 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>IF(ISBLANK(Counts!B8),"-", Counts!B8/234)</f>
@@ -2764,9 +2778,9 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4">
         <f>IF(ISBLANK(Counts!B9),"-", Counts!B9/234)</f>
@@ -2813,9 +2827,9 @@
         <v>g.l.8</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4" t="str">
         <f>IF(ISBLANK(Counts!B10),"-", Counts!B10/234)</f>
@@ -2862,9 +2876,9 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>IF(ISBLANK(Counts!B11),"-", Counts!B11/234)</f>
@@ -2911,9 +2925,9 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>IF(ISBLANK(Counts!B12),"-", Counts!B12/234)</f>
@@ -2960,9 +2974,9 @@
         <v>II.11</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>IF(ISBLANK(Counts!B13),"-", Counts!B13/234)</f>
@@ -3009,9 +3023,9 @@
         <v>II.12</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4">
         <f>IF(ISBLANK(Counts!B14),"-", Counts!B14/234)</f>
@@ -3058,9 +3072,9 @@
         <v>II.13</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>IF(ISBLANK(Counts!B15),"-", Counts!B15/234)</f>
@@ -3107,9 +3121,9 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>IF(ISBLANK(Counts!B16),"-", Counts!B16/234)</f>
@@ -3156,9 +3170,9 @@
         <v>III.15</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>IF(ISBLANK(Counts!B17),"-", Counts!B17/234)</f>
@@ -3205,9 +3219,9 @@
         <v>III.16</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>IF(ISBLANK(Counts!B18),"-", Counts!B18/234)</f>
@@ -3254,9 +3268,9 @@
         <v>III.17</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>IF(ISBLANK(Counts!B19),"-", Counts!B19/234)</f>
@@ -3303,9 +3317,9 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>IF(ISBLANK(Counts!B20),"-", Counts!B20/234)</f>
@@ -3352,9 +3366,9 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>IF(ISBLANK(Counts!B21),"-", Counts!B21/234)</f>
@@ -3401,9 +3415,9 @@
         <v>αC.20</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="4">
         <f>IF(ISBLANK(Counts!B22),"-", Counts!B22/234)</f>
@@ -3450,9 +3464,9 @@
         <v>αC.21</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>IF(ISBLANK(Counts!B23),"-", Counts!B23/234)</f>
@@ -3499,9 +3513,9 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4" t="str">
         <f>IF(ISBLANK(Counts!B24),"-", Counts!B24/234)</f>
@@ -3548,9 +3562,9 @@
         <v>αC.23</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>IF(ISBLANK(Counts!B25),"-", Counts!B25/234)</f>
@@ -3597,9 +3611,9 @@
         <v>αC.24</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4" t="str">
         <f>IF(ISBLANK(Counts!B26),"-", Counts!B26/234)</f>
@@ -3646,9 +3660,9 @@
         <v>αC.25</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="4" t="str">
         <f>IF(ISBLANK(Counts!B27),"-", Counts!B27/234)</f>
@@ -3695,9 +3709,9 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4" t="str">
         <f>IF(ISBLANK(Counts!B28),"-", Counts!B28/234)</f>
@@ -3744,9 +3758,9 @@
         <v>αC.27</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>IF(ISBLANK(Counts!B29),"-", Counts!B29/234)</f>
@@ -3793,9 +3807,9 @@
         <v>αC.28</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>IF(ISBLANK(Counts!B30),"-", Counts!B30/234)</f>
@@ -3842,9 +3856,9 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>IF(ISBLANK(Counts!B31),"-", Counts!B31/234)</f>
@@ -3891,9 +3905,9 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="4">
         <f>IF(ISBLANK(Counts!B32),"-", Counts!B32/234)</f>
@@ -3940,9 +3954,9 @@
         <v>b.l.31</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>IF(ISBLANK(Counts!B33),"-", Counts!B33/234)</f>
@@ -3989,9 +4003,9 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" s="4" t="str">
         <f>IF(ISBLANK(Counts!B34),"-", Counts!B34/234)</f>
@@ -4038,9 +4052,9 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" s="4" t="str">
         <f>IF(ISBLANK(Counts!B35),"-", Counts!B35/234)</f>
@@ -4087,9 +4101,9 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="4">
         <f>IF(ISBLANK(Counts!B36),"-", Counts!B36/234)</f>
@@ -4136,9 +4150,9 @@
         <v>b.l.35</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4" t="str">
         <f>IF(ISBLANK(Counts!B37),"-", Counts!B37/234)</f>
@@ -4185,9 +4199,9 @@
         <v>b.l.36</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" s="4" t="str">
         <f>IF(ISBLANK(Counts!B38),"-", Counts!B38/234)</f>
@@ -4234,9 +4248,9 @@
         <v>b.l.37</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B39" s="4" t="str">
         <f>IF(ISBLANK(Counts!B39),"-", Counts!B39/234)</f>
@@ -4283,9 +4297,9 @@
         <v>IV.38</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" s="4" t="str">
         <f>IF(ISBLANK(Counts!B40),"-", Counts!B40/234)</f>
@@ -4332,9 +4346,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B41" s="4" t="str">
         <f>IF(ISBLANK(Counts!B41),"-", Counts!B41/234)</f>
@@ -4381,9 +4395,9 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4" t="str">
         <f>IF(ISBLANK(Counts!B42),"-", Counts!B42/234)</f>
@@ -4430,9 +4444,9 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B43" s="4" t="str">
         <f>IF(ISBLANK(Counts!B43),"-", Counts!B43/234)</f>
@@ -4479,9 +4493,9 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B44" s="4" t="str">
         <f>IF(ISBLANK(Counts!B44),"-", Counts!B44/234)</f>
@@ -4528,9 +4542,9 @@
         <v>V.43</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B45" s="4" t="str">
         <f>IF(ISBLANK(Counts!B45),"-", Counts!B45/234)</f>
@@ -4577,9 +4591,9 @@
         <v>V.44</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B46" s="4">
         <f>IF(ISBLANK(Counts!B46),"-", Counts!B46/234)</f>
@@ -4626,9 +4640,9 @@
         <v>GK.45</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B47" s="4" t="str">
         <f>IF(ISBLANK(Counts!B47),"-", Counts!B47/234)</f>
@@ -4675,9 +4689,9 @@
         <v>hinge.46</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B48" s="4">
         <f>IF(ISBLANK(Counts!B48),"-", Counts!B48/234)</f>
@@ -4724,9 +4738,9 @@
         <v>hinge.47</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B49" s="4">
         <f>IF(ISBLANK(Counts!B49),"-", Counts!B49/234)</f>
@@ -4773,9 +4787,9 @@
         <v>hinge.48</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B50" s="4" t="str">
         <f>IF(ISBLANK(Counts!B50),"-", Counts!B50/234)</f>
@@ -4822,9 +4836,9 @@
         <v>linker.49</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B51" s="4" t="str">
         <f>IF(ISBLANK(Counts!B51),"-", Counts!B51/234)</f>
@@ -4871,9 +4885,9 @@
         <v>linker.50</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B52" s="4" t="str">
         <f>IF(ISBLANK(Counts!B52),"-", Counts!B52/234)</f>
@@ -4920,9 +4934,9 @@
         <v>linker.51</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B53" s="4" t="str">
         <f>IF(ISBLANK(Counts!B53),"-", Counts!B53/234)</f>
@@ -4969,9 +4983,9 @@
         <v>linker.52</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B54" s="4" t="str">
         <f>IF(ISBLANK(Counts!B54),"-", Counts!B54/234)</f>
@@ -5018,9 +5032,9 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B55" s="4" t="str">
         <f>IF(ISBLANK(Counts!B55),"-", Counts!B55/234)</f>
@@ -5067,9 +5081,9 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B56" s="4" t="str">
         <f>IF(ISBLANK(Counts!B56),"-", Counts!B56/234)</f>
@@ -5116,9 +5130,9 @@
         <v>αD.55</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B57" s="4" t="str">
         <f>IF(ISBLANK(Counts!B57),"-", Counts!B57/234)</f>
@@ -5165,9 +5179,9 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B58" s="4" t="str">
         <f>IF(ISBLANK(Counts!B58),"-", Counts!B58/234)</f>
@@ -5214,9 +5228,9 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B59" s="4" t="str">
         <f>IF(ISBLANK(Counts!B59),"-", Counts!B59/234)</f>
@@ -5263,9 +5277,9 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B60" s="4" t="str">
         <f>IF(ISBLANK(Counts!B60),"-", Counts!B60/234)</f>
@@ -5312,9 +5326,9 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B61" s="4">
         <f>IF(ISBLANK(Counts!B61),"-", Counts!B61/234)</f>
@@ -5361,9 +5375,9 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B62" s="4" t="str">
         <f>IF(ISBLANK(Counts!B62),"-", Counts!B62/234)</f>
@@ -5410,9 +5424,9 @@
         <v>αE.61</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B63" s="4" t="str">
         <f>IF(ISBLANK(Counts!B63),"-", Counts!B63/234)</f>
@@ -5459,9 +5473,9 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B64" s="4" t="str">
         <f>IF(ISBLANK(Counts!B64),"-", Counts!B64/234)</f>
@@ -5508,9 +5522,9 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" s="4" t="str">
         <f>IF(ISBLANK(Counts!B65),"-", Counts!B65/234)</f>
@@ -5557,9 +5571,9 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B66" s="4" t="str">
         <f>IF(ISBLANK(Counts!B66),"-", Counts!B66/234)</f>
@@ -5606,9 +5620,9 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B67" s="4">
         <f>IF(ISBLANK(Counts!B67),"-", Counts!B67/234)</f>
@@ -5655,9 +5669,9 @@
         <v>VI.66</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B68" s="4" t="str">
         <f>IF(ISBLANK(Counts!B68),"-", Counts!B68/234)</f>
@@ -5704,9 +5718,9 @@
         <v>VI.67</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B69" s="4">
         <f>IF(ISBLANK(Counts!B69),"-", Counts!B69/234)</f>
@@ -5753,9 +5767,9 @@
         <v>c.l.68</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B70" s="4" t="str">
         <f>IF(ISBLANK(Counts!B70),"-", Counts!B70/234)</f>
@@ -5802,9 +5816,9 @@
         <v>c.l.69</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B71" s="4" t="str">
         <f>IF(ISBLANK(Counts!B71),"-", Counts!B71/234)</f>
@@ -5851,9 +5865,9 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B72" s="4" t="str">
         <f>IF(ISBLANK(Counts!B72),"-", Counts!B72/234)</f>
@@ -5900,9 +5914,9 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B73" s="4" t="str">
         <f>IF(ISBLANK(Counts!B73),"-", Counts!B73/234)</f>
@@ -5949,9 +5963,9 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B74" s="4" t="str">
         <f>IF(ISBLANK(Counts!B74),"-", Counts!B74/234)</f>
@@ -5998,9 +6012,9 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B75" s="4" t="str">
         <f>IF(ISBLANK(Counts!B75),"-", Counts!B75/234)</f>
@@ -6047,9 +6061,9 @@
         <v>c.l.74</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B76" s="4" t="str">
         <f>IF(ISBLANK(Counts!B76),"-", Counts!B76/234)</f>
@@ -6096,9 +6110,9 @@
         <v>c.l.75</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B77" s="4" t="str">
         <f>IF(ISBLANK(Counts!B77),"-", Counts!B77/234)</f>
@@ -6145,9 +6159,9 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B78" s="4">
         <f>IF(ISBLANK(Counts!B78),"-", Counts!B78/234)</f>
@@ -6194,9 +6208,9 @@
         <v>VII.77</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B79" s="4" t="str">
         <f>IF(ISBLANK(Counts!B79),"-", Counts!B79/234)</f>
@@ -6243,9 +6257,9 @@
         <v>VII.78</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B80" s="4" t="str">
         <f>IF(ISBLANK(Counts!B80),"-", Counts!B80/234)</f>
@@ -6292,9 +6306,9 @@
         <v>VIII.79</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B81" s="4" t="str">
         <f>IF(ISBLANK(Counts!B81),"-", Counts!B81/234)</f>
@@ -6341,9 +6355,9 @@
         <v>xDFG.80</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B82" s="4" t="str">
         <f>IF(ISBLANK(Counts!B82),"-", Counts!B82/234)</f>
@@ -6390,9 +6404,9 @@
         <v>xDFG.81</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B83" s="4">
         <f>IF(ISBLANK(Counts!B83),"-", Counts!B83/234)</f>
@@ -6439,9 +6453,9 @@
         <v>xDFG.82</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B84" s="4" t="str">
         <f>IF(ISBLANK(Counts!B84),"-", Counts!B84/234)</f>
@@ -6488,9 +6502,9 @@
         <v>xDFG.83</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B85" s="4">
         <f>IF(ISBLANK(Counts!B85),"-", Counts!B85/234)</f>
@@ -6537,9 +6551,9 @@
         <v>a.l.84</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B86" s="4" t="str">
         <f>IF(ISBLANK(Counts!B86),"-", Counts!B86/234)</f>

</xml_diff>